<commit_message>
Changes in Class, Camp, Competition and Book a class
</commit_message>
<xml_diff>
--- a/TestDataXls/signin.xlsx
+++ b/TestDataXls/signin.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49990395-35CA-45D7-BB79-0DCF3E9AFFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="signin" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>password</t>
   </si>
@@ -156,9 +155,6 @@
   </si>
   <si>
     <t>genevive@hotmail.com</t>
-  </si>
-  <si>
-    <t>tutor</t>
   </si>
   <si>
     <t>srinivasesaivanan6324@gmail.com</t>
@@ -167,7 +163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,26 +302,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,23 +337,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -550,30 +512,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
     <col min="17" max="17" width="35" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" customWidth="1"/>
-    <col min="19" max="19" width="17.44140625" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
     <col min="21" max="21" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1021,13 +983,13 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>44</v>
@@ -1038,29 +1000,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D12" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D3" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D4" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E2" r:id="rId19" display="Ram@12345" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E16" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E17" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E18" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E19" r:id="rId23" xr:uid="{4D344F2C-AB3D-4C35-8EC5-AF59B32B8107}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D8" r:id="rId8"/>
+    <hyperlink ref="D9" r:id="rId9"/>
+    <hyperlink ref="D10" r:id="rId10"/>
+    <hyperlink ref="D11" r:id="rId11"/>
+    <hyperlink ref="D12" r:id="rId12"/>
+    <hyperlink ref="D13" r:id="rId13"/>
+    <hyperlink ref="D14" r:id="rId14"/>
+    <hyperlink ref="D15" r:id="rId15"/>
+    <hyperlink ref="D3" r:id="rId16"/>
+    <hyperlink ref="D4" r:id="rId17"/>
+    <hyperlink ref="D2" r:id="rId18"/>
+    <hyperlink ref="E2" r:id="rId19" display="Ram@12345"/>
+    <hyperlink ref="E16" r:id="rId20"/>
+    <hyperlink ref="E17" r:id="rId21"/>
+    <hyperlink ref="E18" r:id="rId22"/>
+    <hyperlink ref="E19" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId24"/>

</xml_diff>